<commit_message>
feat(results): add percent new verts and faces
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,220 +790,240 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Mean # of Added Faces</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>79.01206203331419</v>
+          <t>Mean Added Vertices Percentage</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.004448519439807632</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Minimum # of Added Faces</t>
+          <t>Mean # of Added Faces</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>79.01206203331419</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Maximum # of Added Faces</t>
+          <t>Minimum # of Added Faces</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation # of Added Faces</t>
+          <t>Maximum # of Added Faces</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>188.1529141318901</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Mean # of NMEs Before</t>
+          <t>Standard Deviation # of Added Faces</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>96.4744399770247</v>
+        <v>188.1529141318901</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Minimum # of NMEs Before</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
+          <t>Mean Added Faces Percentage</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>0.001385859227250776</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Maximum # of NMEs Before</t>
+          <t>Mean # of NMEs Before</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1929</v>
+        <v>96.4744399770247</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation # of NMEs Before</t>
+          <t>Minimum # of NMEs Before</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>185.8083788599272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Mean # of NMEs After</t>
+          <t>Maximum # of NMEs Before</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Mean Volume</t>
+          <t>Standard Deviation # of NMEs Before</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>255851.5502584722</v>
+        <v>185.8083788599272</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Minimum Volume</t>
+          <t>Mean # of NMEs After</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Maximum Volume</t>
+          <t>Mean Volume</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9533235</v>
+        <v>255851.5502584722</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation Volume</t>
+          <t>Minimum Volume</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>821221.1295896077</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Mean Volume Change</t>
+          <t>Maximum Volume</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>9533235</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time (s)</t>
+          <t>Standard Deviation Volume</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.4485981308076573</v>
+        <v>821221.1295896077</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Minimum Repair Time (s)</t>
+          <t>Mean Volume Change</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.007172200130298734</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Maximum Repair Time (s)</t>
+          <t>Mean Repair Time (s)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10.85378300002776</v>
+        <v>0.4485981308076573</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation Repair Time (s)</t>
+          <t>Minimum Repair Time (s)</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.7843874085008227</v>
+        <v>0.007172200130298734</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Mean Time per Edge Repair (s)</t>
+          <t>Maximum Repair Time (s)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.003736492688821951</v>
+        <v>10.85378300002776</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time Relative to Cuberille Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="n">
-        <v>0.2496465682355021</v>
+          <t>Standard Deviation Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.7843874085008227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time Relative to Surface Nets Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>0.04746570377831323</v>
+          <t>Mean Time per Edge Repair (s)</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.003736492688821951</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
+          <t>Mean Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0.2496465682355021</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Mean Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>0.04746570377831323</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
           <t>Success Rate</t>
         </is>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B30" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(results): add more descriptive statistics for relative performance metrics
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,7 +723,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="76.8" customWidth="1" min="1" max="1"/>
+    <col width="93.59999999999999" customWidth="1" min="1" max="1"/>
     <col width="27.6" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -1010,20 +1010,80 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time Relative to Surface Nets Mesh Generation Time</t>
+          <t>Min Repair Time Relative to Cuberille Mesh Generation Time</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0.04746570377831323</v>
+        <v>0.006947098007963789</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
+          <t>Max Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>2.235620867295733</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>0.2488410955062405</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Mean Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>0.04746570377831323</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Min Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>0.002070496253869231</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Max Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>0.9495387351385597</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>0.07246700117742484</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
           <t>Success Rate</t>
         </is>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B36" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: generate new results with vertices
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -652,16 +652,16 @@
         <v>1364</v>
       </c>
       <c r="C2" t="n">
-        <v>2.035408415396519</v>
+        <v>1.65497067009008</v>
       </c>
       <c r="D2" t="n">
-        <v>0.08139549987390637</v>
+        <v>0.07108120014891028</v>
       </c>
       <c r="E2" t="n">
-        <v>24.58058169996366</v>
+        <v>20.19248209986836</v>
       </c>
       <c r="F2" t="n">
-        <v>3.348428073004833</v>
+        <v>2.75426946832548</v>
       </c>
       <c r="G2" t="n">
         <v>377</v>
@@ -683,16 +683,16 @@
         <v>1741</v>
       </c>
       <c r="C3" t="n">
-        <v>10.33576992102059</v>
+        <v>9.06062797771455</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02492600004188716</v>
+        <v>0.02236719988286495</v>
       </c>
       <c r="E3" t="n">
-        <v>150.4831419999246</v>
+        <v>131.3533709999174</v>
       </c>
       <c r="F3" t="n">
-        <v>17.33433211760955</v>
+        <v>15.41417822432034</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -750,340 +750,490 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Mean # of Added Vertices</t>
+          <t>Number with NMVs</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>119.4870763928777</v>
+        <v>899</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Minimum # of Added Vertices</t>
+          <t>Mean # of Added Vertices</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>142.4537622056289</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Maximum # of Added Vertices</t>
+          <t>Minimum # of Added Vertices</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2617</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation # of Added Vertices</t>
+          <t>Maximum # of Added Vertices</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>237.2237411504864</v>
+        <v>3302</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Mean Added Vertices Percentage</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>0.004448519439807632</v>
+          <t>Standard Deviation # of Added Vertices</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>288.0614479167753</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Mean # of Added Faces</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>79.01206203331419</v>
+          <t>Mean Added Vertices Percentage</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.005294163506840346</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Minimum # of Added Faces</t>
+          <t>Mean # of Added Faces</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>79.01206203331419</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Maximum # of Added Faces</t>
+          <t>Minimum # of Added Faces</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation # of Added Faces</t>
+          <t>Maximum # of Added Faces</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>188.1529141318901</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Mean Added Faces Percentage</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>0.001385859227250776</v>
+          <t>Standard Deviation # of Added Faces</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>188.1529141318901</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Mean # of NMEs Before</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>96.4744399770247</v>
+          <t>Mean Added Faces Percentage</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0.001385859227250776</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Minimum # of NMEs Before</t>
+          <t>Mean # of NMEs Before</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>96.4744399770247</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Maximum # of NMEs Before</t>
+          <t>Minimum # of NMEs Before</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation # of NMEs Before</t>
+          <t>Maximum # of NMEs Before</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>185.8083788599272</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Mean # of NMEs After</t>
+          <t>Standard Deviation # of NMEs Before</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>185.8083788599272</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Mean Volume</t>
+          <t>Mean # of NMEs After</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>255851.5502584722</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Minimum Volume</t>
+          <t>Mean # of NMVs Before</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>359</v>
+        <v>20.98506605399196</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Maximum Volume</t>
+          <t>Minimum # of NMVs Before</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>9533235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation Volume</t>
+          <t>Maximum # of NMVs Before</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>821221.1295896077</v>
+        <v>624</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Mean Volume Change</t>
+          <t>Standard Deviation # of NMVs Before</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>47.63407337631442</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time (s)</t>
+          <t>Mean # of NMVs After</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.4485981308076573</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Minimum Repair Time (s)</t>
+          <t>Mean Volume</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.007172200130298734</v>
+        <v>255851.5502584722</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Maximum Repair Time (s)</t>
+          <t>Minimum Volume</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10.85378300002776</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation Repair Time (s)</t>
+          <t>Maximum Volume</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.7843874085008227</v>
+        <v>9533235</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Mean Time per Edge Repair (s)</t>
+          <t>Standard Deviation Volume</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.003736492688821951</v>
+        <v>821221.1295896077</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time Relative to Cuberille Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="n">
-        <v>0.2496465682355021</v>
+          <t>Mean Volume Change</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Min Repair Time Relative to Cuberille Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>0.006947098007963789</v>
+          <t>Edges Mean Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.3515774603990346</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Max Repair Time Relative to Cuberille Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="n">
-        <v>2.235620867295733</v>
+          <t>Edges Minimum Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.004164200043305755</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation Repair Time Relative to Cuberille Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>0.2488410955062405</v>
+          <t>Edges Maximum Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>9.458849499933422</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Mean Repair Time Relative to Surface Nets Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>0.04746570377831323</v>
+          <t>Edges Standard Deviation Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.6631316613533466</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Min Repair Time Relative to Surface Nets Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>0.002070496253869231</v>
+          <t>Vertices Mean Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.04517836039818542</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Max Repair Time Relative to Surface Nets Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="n">
-        <v>0.9495387351385597</v>
+          <t>Vertices Minimum Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.001613700063899159</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation Repair Time Relative to Surface Nets Mesh Generation Time</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="n">
-        <v>0.07246700117742484</v>
+          <t>Vertices Maximum Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.6624916999135166</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
+          <t>Vertices Standard Deviation Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.072328306924953</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Total Mean Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.3931456988573239</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Total Minimum Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.006134700030088425</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Total Maximum Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>9.736861299956217</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Total Standard Deviation Repair Time (s)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.7068926608883704</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Mean Time per Edge Repair (s)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.002928381819091518</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Mean Time per Vertex Repair (s)</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.001111683207827253</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>Mean Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>0.2649837108516612</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Min Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>0.009768309511608573</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>Max Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>2.409305717513604</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation Repair Time Relative to Cuberille Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>0.2651064129487007</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Mean Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>0.0482680616815102</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>Min Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>0.001917253643808106</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>Max Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>0.7558407705526704</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation Repair Time Relative to Surface Nets Mesh Generation Time</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>0.07401962938896677</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
           <t>Success Rate</t>
         </is>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B51" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>